<commit_message>
Best Practice Summary implemented
RiskBox handles better floating point operations that in borwser JavaScript.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" state="visible" r:id="rId2"/>
@@ -2627,7 +2627,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2713,8 +2713,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2915,14 +2915,14 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -9539,16 +9539,16 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -10852,11 +10852,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -14531,16 +14531,16 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.2"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>

</xml_diff>